<commit_message>
worked with the aci fit code some more
</commit_message>
<xml_diff>
--- a/Inputs/2022-08-11-0949_walkup_aci_clean.xlsx
+++ b/Inputs/2022-08-11-0949_walkup_aci_clean.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maquellegarcia/Desktop/MNG_6400_cleaning/Clean/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmel\Desktop\DAT_proj\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20FACB7-83F7-7141-890C-B6DB5E1EB534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCA74E2-71E9-4F7E-914F-D9F87A5452F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="1" r:id="rId1"/>
     <sheet name="Remarks" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="425">
   <si>
     <t>File opened</t>
   </si>
@@ -1305,6 +1303,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>exclude</t>
   </si>
 </sst>
 </file>
@@ -1682,16 +1683,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:IN27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HP1" workbookViewId="0">
-      <selection activeCell="IN17" sqref="IN17:IN27"/>
+    <sheetView tabSelected="1" topLeftCell="HR9" workbookViewId="0">
+      <selection activeCell="IN18" sqref="IN18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:248" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>4</v>
       </c>
@@ -1710,7 +1711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1745,7 +1746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:248" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1777,7 +1778,7 @@
         <v>96.9</v>
       </c>
     </row>
-    <row r="6" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:248" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>0</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:248" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>51</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>0.2175</v>
       </c>
     </row>
-    <row r="10" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:248" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0</v>
       </c>
@@ -1948,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:248" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>-6276</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -3486,7 +3487,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="16" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:248" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>345</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -4829,10 +4830,10 @@
         <v>100.37</v>
       </c>
       <c r="IN17" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
-    <row r="18" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="19" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -6392,7 +6393,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="20" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -7172,7 +7173,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="21" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -7952,7 +7953,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="22" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6</v>
       </c>
@@ -8732,7 +8733,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="23" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7</v>
       </c>
@@ -9512,7 +9513,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
@@ -10292,7 +10293,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>9</v>
       </c>
@@ -11072,7 +11073,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -11852,7 +11853,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="27" spans="1:248" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:248" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>11</v>
       </c>
@@ -12643,9 +12644,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12653,7 +12654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -12661,7 +12662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -12669,7 +12670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -12677,7 +12678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -12685,7 +12686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -12693,7 +12694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -12701,7 +12702,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -12709,7 +12710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -12717,7 +12718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -12725,7 +12726,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -12733,7 +12734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -12741,7 +12742,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -12749,7 +12750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -12757,7 +12758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -12765,7 +12766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>

</xml_diff>